<commit_message>
random side select v1
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Start</t>
   </si>
@@ -37,130 +37,175 @@
     <t>MM Traveled</t>
   </si>
   <si>
-    <t>(327, 140)</t>
-  </si>
-  <si>
-    <t>(456, 155)</t>
-  </si>
-  <si>
-    <t>129.86916493148016</t>
-  </si>
-  <si>
-    <t>0:00:00.401500</t>
-  </si>
-  <si>
-    <t>[[356, 145, datetime.timedelta(microseconds=81782), 177.0588625707253], [422, 151, datetime.timedelta(microseconds=162917), 103.32334986645584, -452.59557139076617], [448, 155, datetime.timedelta(microseconds=243749), 27.412201857183742, -311.43162847548956], [456, 156, datetime.timedelta(microseconds=322532), 6.349179207234729, -65.3052182417528]]</t>
-  </si>
-  <si>
-    <t>2022-07-12 11:39:46.390465</t>
-  </si>
-  <si>
-    <t>32.986767892595964</t>
-  </si>
-  <si>
-    <t>(312, 134)</t>
-  </si>
-  <si>
-    <t>(311, 133)</t>
+    <t>(314, 126)</t>
+  </si>
+  <si>
+    <t>(316, 129)</t>
+  </si>
+  <si>
+    <t>3.6055512754639896</t>
+  </si>
+  <si>
+    <t>0:00:00.202427</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:53:32.918456</t>
+  </si>
+  <si>
+    <t>2.2156694128254517</t>
+  </si>
+  <si>
+    <t>(331, 143)</t>
+  </si>
+  <si>
+    <t>(390, 144)</t>
+  </si>
+  <si>
+    <t>59.008473967727724</t>
+  </si>
+  <si>
+    <t>0:00:01.429046</t>
+  </si>
+  <si>
+    <t>[[327, 141, datetime.timedelta(microseconds=204453), 47.523651564219136], [342, 134, datetime.timedelta(microseconds=431919), 23.550832227843234, -55.50304417350453], [378, 140, datetime.timedelta(microseconds=649382), 34.53704307117837, 16.917947900211484], [392, 150, datetime.timedelta(microseconds=845439), 12.50537915515944, -26.05943647740278], [392, 147, datetime.timedelta(seconds=1, microseconds=52929), 34.83059168124798, 421.7954717846274], [391, 145, datetime.timedelta(seconds=1, microseconds=238470), 5.762149695081819, -121.89559267902112]]</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:53:41.295857</t>
+  </si>
+  <si>
+    <t>36.261659002748814</t>
+  </si>
+  <si>
+    <t>(315, 138)</t>
+  </si>
+  <si>
+    <t>(316, 137)</t>
   </si>
   <si>
     <t>1.4142135623730951</t>
   </si>
   <si>
-    <t>0:00:00.079332</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>2022-07-12 11:39:48.454715</t>
-  </si>
-  <si>
-    <t>0.3592102448427662</t>
-  </si>
-  <si>
-    <t>(312, 131)</t>
-  </si>
-  <si>
-    <t>(312, 133)</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>0:00:00.082781</t>
-  </si>
-  <si>
-    <t>2022-07-12 11:39:49.209948</t>
-  </si>
-  <si>
-    <t>0.508</t>
-  </si>
-  <si>
-    <t>(311, 134)</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>0:00:00.086770</t>
-  </si>
-  <si>
-    <t>2022-07-12 11:39:50.425698</t>
-  </si>
-  <si>
-    <t>0.254</t>
-  </si>
-  <si>
-    <t>(312, 137)</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>0:00:00.243449</t>
-  </si>
-  <si>
-    <t>[[311, 131, datetime.timedelta(microseconds=79767), 56.335561413746916], [311, 135, datetime.timedelta(microseconds=162055), 6.269476412329148, -308.94501867525076]]</t>
-  </si>
-  <si>
-    <t>2022-07-12 11:39:50.787119</t>
-  </si>
-  <si>
-    <t>1.016</t>
-  </si>
-  <si>
-    <t>(312, 132)</t>
-  </si>
-  <si>
-    <t>(313, 133)</t>
-  </si>
-  <si>
-    <t>0:00:00.095895</t>
-  </si>
-  <si>
-    <t>2022-07-12 11:39:51.555655</t>
-  </si>
-  <si>
-    <t>(299, 144)</t>
-  </si>
-  <si>
-    <t>(157, 142)</t>
-  </si>
-  <si>
-    <t>142.01408380861386</t>
-  </si>
-  <si>
-    <t>0:00:00.485975</t>
-  </si>
-  <si>
-    <t>[[259, 155, datetime.timedelta(microseconds=79029), 133.33300439645325], [208, 160, datetime.timedelta(microseconds=157817), 82.47594380151733, -322.2533731786558], [161, 147, datetime.timedelta(microseconds=239598), 51.69594197647893, -128.46518679220364], [154, 142, datetime.timedelta(microseconds=320428), 6.818975301249664, -140.05319970548535], [157, 143, datetime.timedelta(microseconds=401166), 2.0022098724287916, -12.00691341943453]]</t>
-  </si>
-  <si>
-    <t>2022-07-12 11:39:53.138550</t>
-  </si>
-  <si>
-    <t>36.071577287387925</t>
+    <t>0:00:00.234374</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:53:47.042532</t>
+  </si>
+  <si>
+    <t>0.8690570439744343</t>
+  </si>
+  <si>
+    <t>(312, 128)</t>
+  </si>
+  <si>
+    <t>(314, 133)</t>
+  </si>
+  <si>
+    <t>5.385164807134505</t>
+  </si>
+  <si>
+    <t>0:00:00.222741</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:53:56.245652</t>
+  </si>
+  <si>
+    <t>3.3092706314810427</t>
+  </si>
+  <si>
+    <t>(317, 116)</t>
+  </si>
+  <si>
+    <t>(269, 100)</t>
+  </si>
+  <si>
+    <t>50.59644256269407</t>
+  </si>
+  <si>
+    <t>0:00:02.109195</t>
+  </si>
+  <si>
+    <t>[[316, 85, datetime.timedelta(microseconds=206448), 140.02749292785086], [309, 87, datetime.timedelta(microseconds=420876), 10.629603370327901, -307.4489625389021], [275, 97, datetime.timedelta(microseconds=645305), 33.749168377149104, 35.82734521942524], [268, 103, datetime.timedelta(microseconds=867770), 6.5288714421291765, -31.368100919621476], [265, 101, datetime.timedelta(seconds=1, microseconds=64247), 34.48673732353965, 435.1622002803318], [268, 103, datetime.timedelta(seconds=1, microseconds=267745), 8.275297065586479, -97.8970298528569], [271, 100, datetime.timedelta(seconds=1, microseconds=477178), 5.4637286964682, -5.8920745908618555], [271, 103, datetime.timedelta(seconds=1, microseconds=690606), 2.669464770211632, -4.046104329033586], [269, 99, datetime.timedelta(seconds=1, microseconds=905660), 3.034471739474331, 0.40302869648952055]]</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:54:03.428435</t>
+  </si>
+  <si>
+    <t>31.092330026429746</t>
+  </si>
+  <si>
+    <t>(289, 143)</t>
+  </si>
+  <si>
+    <t>(225, 141)</t>
+  </si>
+  <si>
+    <t>64.03124237432849</t>
+  </si>
+  <si>
+    <t>0:00:01.275191</t>
+  </si>
+  <si>
+    <t>[[261, 141, datetime.timedelta(microseconds=211903), 155.89963640477768], [254, 146, datetime.timedelta(microseconds=430346), 12.283761493726956, -333.72187707344955], [250, 146, datetime.timedelta(microseconds=631394), 3.8930755061483517, -13.289144318093939], [231, 146, datetime.timedelta(microseconds=834862), 13.985313083614901, 12.088509930343637], [225, 140, datetime.timedelta(seconds=1, microseconds=56742), 91.89563751447967, 1373.0627124680973]]</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:54:21.839108</t>
+  </si>
+  <si>
+    <t>39.34823120099863</t>
+  </si>
+  <si>
+    <t>(314, 132)</t>
+  </si>
+  <si>
+    <t>(314, 137)</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>0:00:00.205961</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:54:26.542371</t>
+  </si>
+  <si>
+    <t>3.0725806451612905</t>
+  </si>
+  <si>
+    <t>(316, 128)</t>
+  </si>
+  <si>
+    <t>(316, 135)</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>0:00:00.203456</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:54:28.700378</t>
+  </si>
+  <si>
+    <t>4.301612903225807</t>
+  </si>
+  <si>
+    <t>(315, 134)</t>
+  </si>
+  <si>
+    <t>2.23606797749979</t>
+  </si>
+  <si>
+    <t>0:00:00.205910</t>
+  </si>
+  <si>
+    <t>2022-07-12 14:54:31.667419</t>
+  </si>
+  <si>
+    <t>1.3740998377861613</t>
   </si>
   <si>
     <t>Name:</t>
@@ -498,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -587,7 +632,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -601,99 +646,145 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
target hit miss v1
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
   <si>
     <t>Start</t>
   </si>
@@ -37,94 +37,298 @@
     <t>MM Traveled</t>
   </si>
   <si>
-    <t>(364, 189)</t>
-  </si>
-  <si>
-    <t>(420, 186)</t>
-  </si>
-  <si>
-    <t>56.080299571239806</t>
-  </si>
-  <si>
-    <t>0:00:00.416525</t>
-  </si>
-  <si>
-    <t>[[380, 185, datetime.timedelta(microseconds=100726), 50.60866481036415], [406, 184, datetime.timedelta(microseconds=204481), 53.8671303632033, 15.935297425380133], [419, 188, datetime.timedelta(microseconds=308811), 18.645565892076398, -114.0554075830424]]</t>
-  </si>
-  <si>
-    <t>2022-07-14 15:13:19.237900</t>
-  </si>
-  <si>
-    <t>23.74066015182485</t>
-  </si>
-  <si>
-    <t>(348, 197)</t>
-  </si>
-  <si>
-    <t>(347, 195)</t>
-  </si>
-  <si>
-    <t>2.23606797749979</t>
-  </si>
-  <si>
-    <t>0:00:00.099874</t>
+    <t>Target Hit</t>
+  </si>
+  <si>
+    <t>Target Center</t>
+  </si>
+  <si>
+    <t>Distance From Center</t>
+  </si>
+  <si>
+    <t>(367, 185)</t>
+  </si>
+  <si>
+    <t>(466, 194)</t>
+  </si>
+  <si>
+    <t>99.40824915468535</t>
+  </si>
+  <si>
+    <t>0:00:00.386083</t>
+  </si>
+  <si>
+    <t>[[403, 188, datetime.timedelta(microseconds=70846), 380.29985657714883], [434, 191, datetime.timedelta(microseconds=145646), 98.15991840280543, -1937.16228509086], [463, 195, datetime.timedelta(microseconds=239427), 56.12601013759703, -175.56043497687563], [467, 195, datetime.timedelta(microseconds=312232), 5.880705944020002, -160.9229809679246]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:37:52.998791</t>
+  </si>
+  <si>
+    <t>45.63197943124713</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>(1460.5, 540.0)</t>
+  </si>
+  <si>
+    <t>1052.9702037569725</t>
+  </si>
+  <si>
+    <t>(319, 183)</t>
+  </si>
+  <si>
+    <t>(320, 183)</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>0:00:00.079446</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>2022-07-14 15:13:22.817329</t>
-  </si>
-  <si>
-    <t>0.946602110474911</t>
-  </si>
-  <si>
-    <t>(352, 194)</t>
+    <t>2022-07-15 11:37:54.983948</t>
+  </si>
+  <si>
+    <t>0.45903614457831327</t>
+  </si>
+  <si>
+    <t>miss</t>
+  </si>
+  <si>
+    <t>(458.5, 540.0)</t>
+  </si>
+  <si>
+    <t>382.92460093339525</t>
+  </si>
+  <si>
+    <t>(305, 183)</t>
+  </si>
+  <si>
+    <t>(149, 198)</t>
+  </si>
+  <si>
+    <t>156.7194946393077</t>
+  </si>
+  <si>
+    <t>0:00:00.472846</t>
+  </si>
+  <si>
+    <t>[[276, 187, datetime.timedelta(microseconds=74800), 426.2790058614439], [218, 193, datetime.timedelta(microseconds=165257), 161.96697731602276, -1599.3998955894226], [186, 195, datetime.timedelta(microseconds=241022), 61.064211660294504, -418.64545832217914], [164, 195, datetime.timedelta(microseconds=318651), 31.692337951937677, -92.1756834541766], [151, 197, datetime.timedelta(microseconds=394795), 15.293197286513069, -41.53836969927332]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:37:56.272099</t>
+  </si>
+  <si>
+    <t>71.93991259948945</t>
+  </si>
+  <si>
+    <t>461.2529132699326</t>
+  </si>
+  <si>
+    <t>(319, 180)</t>
+  </si>
+  <si>
+    <t>(318, 181)</t>
+  </si>
+  <si>
+    <t>1.4142135623730951</t>
+  </si>
+  <si>
+    <t>0:00:00.073443</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:37:58.662731</t>
+  </si>
+  <si>
+    <t>0.6491751412821076</t>
+  </si>
+  <si>
+    <t>385.51426692147203</t>
+  </si>
+  <si>
+    <t>(313, 180)</t>
+  </si>
+  <si>
+    <t>(174, 192)</t>
+  </si>
+  <si>
+    <t>139.51702405083043</t>
+  </si>
+  <si>
+    <t>0:00:00.463822</t>
+  </si>
+  <si>
+    <t>[[285, 185, datetime.timedelta(microseconds=76799), 360.41533029942434], [248, 187, datetime.timedelta(microseconds=153599), 110.73725750599425, -1625.518869220699], [215, 189, datetime.timedelta(microseconds=229467), 66.13581754055511, -194.36973493111927], [185, 191, datetime.timedelta(microseconds=305537), 45.171788751158914, -68.61371548910998], [176, 193, datetime.timedelta(microseconds=383353), 11.039705291060942, -89.03564980604814]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:37:59.897075</t>
+  </si>
+  <si>
+    <t>64.04335682333301</t>
+  </si>
+  <si>
+    <t>449.49332586813784</t>
   </si>
   <si>
     <t>0.0</t>
   </si>
   <si>
-    <t>0:00:00.099770</t>
-  </si>
-  <si>
-    <t>2022-07-14 15:13:24.877388</t>
-  </si>
-  <si>
-    <t>(345, 194)</t>
-  </si>
-  <si>
-    <t>0:00:00.099734</t>
-  </si>
-  <si>
-    <t>2022-07-14 15:13:25.801916</t>
-  </si>
-  <si>
-    <t>(372, 194)</t>
-  </si>
-  <si>
-    <t>(454, 198)</t>
-  </si>
-  <si>
-    <t>82.09750300709516</t>
-  </si>
-  <si>
-    <t>0:00:00.802404</t>
-  </si>
-  <si>
-    <t>[[390, 195, datetime.timedelta(microseconds=99732), 76.52258251847061], [411, 190, datetime.timedelta(microseconds=207604), 44.01895290079846, -156.56552676091096], [422, 192, datetime.timedelta(microseconds=328282), 14.417514674501055, -90.17076241249111], [435, 194, datetime.timedelta(microseconds=441286), 12.617850234856533, -4.078226908727043], [450, 196, datetime.timedelta(microseconds=555978), 11.52239078826583, -1.9703287658697], [455, 197, datetime.timedelta(microseconds=674662), 3.199505719042937, -12.33637742932445]]</t>
-  </si>
-  <si>
-    <t>2022-07-14 15:13:30.229620</t>
-  </si>
-  <si>
-    <t>34.75460960633695</t>
+    <t>0:00:00.076295</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:02.050585</t>
+  </si>
+  <si>
+    <t>1202.6455213403492</t>
+  </si>
+  <si>
+    <t>(308, 180)</t>
+  </si>
+  <si>
+    <t>(150, 193)</t>
+  </si>
+  <si>
+    <t>158.5339080449353</t>
+  </si>
+  <si>
+    <t>0:00:00.484518</t>
+  </si>
+  <si>
+    <t>[[266, 185, datetime.timedelta(microseconds=83380), 436.1752883372185], [227, 188, datetime.timedelta(microseconds=157198), 114.22090120013831, -2048.081954840902], [192, 190, datetime.timedelta(microseconds=232980), 69.07234234353886, -193.78727297020967], [159, 193, datetime.timedelta(microseconds=323911), 46.959380232272785, -68.26863586375912], [150, 194, datetime.timedelta(microseconds=401996), 10.340274732789274, -91.09320863760712]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:03.316366</t>
+  </si>
+  <si>
+    <t>72.77279393387994</t>
+  </si>
+  <si>
+    <t>464.3072797189379</t>
+  </si>
+  <si>
+    <t>(313, 182)</t>
+  </si>
+  <si>
+    <t>(314, 182)</t>
+  </si>
+  <si>
+    <t>0:00:00.076830</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:05.536349</t>
+  </si>
+  <si>
+    <t>1201.0937723591776</t>
+  </si>
+  <si>
+    <t>(293, 184)</t>
+  </si>
+  <si>
+    <t>(146, 194)</t>
+  </si>
+  <si>
+    <t>147.33974345029927</t>
+  </si>
+  <si>
+    <t>0:00:00.397434</t>
+  </si>
+  <si>
+    <t>[[259, 188, datetime.timedelta(microseconds=81780), 485.3594249689224], [204, 190, datetime.timedelta(microseconds=158427), 159.46571393008367, -2057.0591568283107], [171, 193, datetime.timedelta(microseconds=236095), 64.42601414860844, -402.5485494460926], [148, 194, datetime.timedelta(microseconds=315946), 33.448138797070094, -98.04800615148902]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:06.882281</t>
+  </si>
+  <si>
+    <t>67.63426777658316</t>
+  </si>
+  <si>
+    <t>466.2319701607774</t>
+  </si>
+  <si>
+    <t>(317, 181)</t>
+  </si>
+  <si>
+    <t>0:00:00.079951</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:08.920807</t>
+  </si>
+  <si>
+    <t>1198.529619992764</t>
+  </si>
+  <si>
+    <t>(333, 182)</t>
+  </si>
+  <si>
+    <t>(474, 193)</t>
+  </si>
+  <si>
+    <t>141.42842712835352</t>
+  </si>
+  <si>
+    <t>0:00:00.464583</t>
+  </si>
+  <si>
+    <t>[[360, 183, datetime.timedelta(microseconds=74818), 95.24656232900384], [395, 183, datetime.timedelta(microseconds=149613), 107.3854882947402, 81.13550270187993], [447, 189, datetime.timedelta(microseconds=238361), 100.80613549637583, -27.602471874024562], [469, 192, datetime.timedelta(microseconds=310170), 32.860226519998136, -219.0602217376848], [474, 194, datetime.timedelta(microseconds=381521), 6.479290238245965, -69.14674757549956]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:10.198782</t>
+  </si>
+  <si>
+    <t>64.92075992277434</t>
+  </si>
+  <si>
+    <t>1045.7491333967241</t>
+  </si>
+  <si>
+    <t>(310, 179)</t>
+  </si>
+  <si>
+    <t>(309, 180)</t>
+  </si>
+  <si>
+    <t>0:00:00.076798</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:12.159897</t>
+  </si>
+  <si>
+    <t>389.8079655420089</t>
+  </si>
+  <si>
+    <t>(345, 179)</t>
+  </si>
+  <si>
+    <t>(472, 189)</t>
+  </si>
+  <si>
+    <t>127.39309243440165</t>
+  </si>
+  <si>
+    <t>0:00:00.457903</t>
+  </si>
+  <si>
+    <t>[[391, 182, datetime.timedelta(microseconds=80031), 264.4040523324765], [420, 184, datetime.timedelta(microseconds=158750), 84.05460349155837, -1136.059520257752], [446, 187, datetime.timedelta(microseconds=234380), 51.25917583209242, -139.92417296469816], [466, 189, datetime.timedelta(microseconds=309221), 29.837922771163118, -69.2748974388198], [471, 190, datetime.timedelta(microseconds=383980), 6.095719200607372, -61.831875541840056]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 11:38:13.511245</t>
+  </si>
+  <si>
+    <t>58.47803399699642</t>
+  </si>
+  <si>
+    <t>1048.9677068432563</t>
   </si>
   <si>
     <t>Subject Code:</t>
   </si>
   <si>
-    <t>1</t>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -456,13 +660,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,128 +688,438 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="I13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
+      <c r="J13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added number of trials
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Start</t>
   </si>
@@ -46,58 +46,88 @@
     <t>Distance From Center</t>
   </si>
   <si>
-    <t>(992, 552)</t>
-  </si>
-  <si>
-    <t>(1261, 559)</t>
-  </si>
-  <si>
-    <t>269.09106265351886</t>
-  </si>
-  <si>
-    <t>0:00:00.548000</t>
-  </si>
-  <si>
-    <t>[[1030, 554, datetime.timedelta(microseconds=78187), 36.67798912202631], [1050, 557, datetime.timedelta(microseconds=149005), 55.60359089166522, 127.01319935330298], [1083, 559, datetime.timedelta(microseconds=232001), 58.37975273915533, 11.966163281581151], [1243, 559, datetime.timedelta(microseconds=316999), 206.77789865827398, 468.1344291910027], [1253, 559, datetime.timedelta(microseconds=393000), 10.424361815644751, -499.62732021025255], [1261, 559, datetime.timedelta(microseconds=470043), 6.972594751626361, -7.343513389239686]]</t>
-  </si>
-  <si>
-    <t>2022-07-15 14:52:35.139728</t>
-  </si>
-  <si>
-    <t>110.24053211934482</t>
+    <t>(664, 549)</t>
+  </si>
+  <si>
+    <t>(531, 552)</t>
+  </si>
+  <si>
+    <t>133.0338302838793</t>
+  </si>
+  <si>
+    <t>0:00:00.236185</t>
+  </si>
+  <si>
+    <t>[[541, 554, datetime.timedelta(microseconds=77279), 2727.850365128794], [531, 552, datetime.timedelta(microseconds=160398), 26.915359635668104, -16838.956879095287]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 15:13:22.015893</t>
+  </si>
+  <si>
+    <t>56.317654820175576</t>
+  </si>
+  <si>
+    <t>miss</t>
+  </si>
+  <si>
+    <t>(645.5, 540.0)</t>
+  </si>
+  <si>
+    <t>115.12710367241937</t>
+  </si>
+  <si>
+    <t>(1083, 541)</t>
+  </si>
+  <si>
+    <t>(1454, 549)</t>
+  </si>
+  <si>
+    <t>371.0862433451286</t>
+  </si>
+  <si>
+    <t>0:00:00.500964</t>
+  </si>
+  <si>
+    <t>[[1151, 549, datetime.timedelta(microseconds=77005), 637.4467985693265], [1180, 549, datetime.timedelta(microseconds=151974), 80.78136172415458, -3662.8991593639166], [1329, 559, datetime.timedelta(microseconds=234724), 269.33149240499637, 803.2844135275549], [1452, 557, datetime.timedelta(microseconds=322965), 161.24621248094928, -334.6656136858393], [1452, 552, datetime.timedelta(microseconds=413939), 5.113474851769626, -377.18779247468746]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 15:13:27.348214</t>
+  </si>
+  <si>
+    <t>157.09317634943778</t>
+  </si>
+  <si>
+    <t>(1273.5, 540.0)</t>
+  </si>
+  <si>
+    <t>180.7242374447877</t>
+  </si>
+  <si>
+    <t>(1038, 523)</t>
+  </si>
+  <si>
+    <t>(1287, 486)</t>
+  </si>
+  <si>
+    <t>251.73398658107334</t>
+  </si>
+  <si>
+    <t>0:00:00.621378</t>
+  </si>
+  <si>
+    <t>[[1067, 512, datetime.timedelta(microseconds=81938), 160.24505742125305], [1114, 510, datetime.timedelta(microseconds=164523), 121.04491592989531, -238.26541876429278], [1216, 507, datetime.timedelta(microseconds=250489), 172.4573631309366, 205.24832308421253], [1227, 499, datetime.timedelta(microseconds=346485), 16.618196599269826, -449.77175500141936], [1253, 494, datetime.timedelta(microseconds=442484), 25.330508243596956, 19.689551812782227], [1287, 489, datetime.timedelta(microseconds=538484), 27.016843771710054, 3.131635346849856]]</t>
+  </si>
+  <si>
+    <t>2022-07-15 15:13:32.185694</t>
+  </si>
+  <si>
+    <t>106.56738765265439</t>
   </si>
   <si>
     <t>hit</t>
   </si>
   <si>
-    <t>(1273.5, 540.0)</t>
-  </si>
-  <si>
-    <t>22.743130831088315</t>
-  </si>
-  <si>
-    <t>(1023, 554)</t>
-  </si>
-  <si>
-    <t>(1258, 562)</t>
-  </si>
-  <si>
-    <t>235.1361307838504</t>
-  </si>
-  <si>
-    <t>0:00:00.470306</t>
-  </si>
-  <si>
-    <t>[[1083, 557, datetime.timedelta(microseconds=93662), 262.7677370553693], [1114, 557, datetime.timedelta(microseconds=166907), 76.09027781938444, -1118.4519477073154], [1164, 562, datetime.timedelta(microseconds=237943), 86.51666805280914, 43.818856757394414], [1250, 559, datetime.timedelta(microseconds=316941), 111.2310750462082, 77.97794224603024], [1261, 562, datetime.timedelta(microseconds=392267), 11.907810898352933, -253.2032114550938]]</t>
-  </si>
-  <si>
-    <t>2022-07-15 14:52:45.029205</t>
-  </si>
-  <si>
-    <t>96.32996325660967</t>
-  </si>
-  <si>
-    <t>26.911893281595777</t>
+    <t>55.66192594583842</t>
   </si>
   <si>
     <t>Subject Code:</t>
@@ -435,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -531,18 +561,50 @@
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed tkinter weird gui
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Start</t>
   </si>
@@ -46,88 +46,112 @@
     <t>Distance From Center</t>
   </si>
   <si>
-    <t>(664, 549)</t>
-  </si>
-  <si>
-    <t>(531, 552)</t>
-  </si>
-  <si>
-    <t>133.0338302838793</t>
-  </si>
-  <si>
-    <t>0:00:00.236185</t>
-  </si>
-  <si>
-    <t>[[541, 554, datetime.timedelta(microseconds=77279), 2727.850365128794], [531, 552, datetime.timedelta(microseconds=160398), 26.915359635668104, -16838.956879095287]]</t>
-  </si>
-  <si>
-    <t>2022-07-15 15:13:22.015893</t>
-  </si>
-  <si>
-    <t>56.317654820175576</t>
+    <t>(726, 347)</t>
+  </si>
+  <si>
+    <t>(840, 341)</t>
+  </si>
+  <si>
+    <t>114.15778554264269</t>
+  </si>
+  <si>
+    <t>0:00:00.242883</t>
+  </si>
+  <si>
+    <t>[[837, 339, datetime.timedelta(microseconds=108936), 203.11786467979857]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 13:22:23.360727</t>
+  </si>
+  <si>
+    <t>35.07590023527973</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>(893.5, 360.0)</t>
+  </si>
+  <si>
+    <t>56.77367347635698</t>
+  </si>
+  <si>
+    <t>(614, 327)</t>
+  </si>
+  <si>
+    <t>(460, 325)</t>
+  </si>
+  <si>
+    <t>154.01298646542764</t>
+  </si>
+  <si>
+    <t>0:00:00.502601</t>
+  </si>
+  <si>
+    <t>[[563, 322, datetime.timedelta(microseconds=147599), 436.052055827327], [487, 321, datetime.timedelta(microseconds=254267), 91.84689421110689, -1353.7154314803738], [462, 325, datetime.timedelta(microseconds=387026), 20.099819797663816, -185.3805026366267]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 13:22:30.539934</t>
+  </si>
+  <si>
+    <t>47.321732131716075</t>
   </si>
   <si>
     <t>miss</t>
   </si>
   <si>
-    <t>(645.5, 540.0)</t>
-  </si>
-  <si>
-    <t>115.12710367241937</t>
-  </si>
-  <si>
-    <t>(1083, 541)</t>
-  </si>
-  <si>
-    <t>(1454, 549)</t>
-  </si>
-  <si>
-    <t>371.0862433451286</t>
-  </si>
-  <si>
-    <t>0:00:00.500964</t>
-  </si>
-  <si>
-    <t>[[1151, 549, datetime.timedelta(microseconds=77005), 637.4467985693265], [1180, 549, datetime.timedelta(microseconds=151974), 80.78136172415458, -3662.8991593639166], [1329, 559, datetime.timedelta(microseconds=234724), 269.33149240499637, 803.2844135275549], [1452, 557, datetime.timedelta(microseconds=322965), 161.24621248094928, -334.6656136858393], [1452, 552, datetime.timedelta(microseconds=413939), 5.113474851769626, -377.18779247468746]]</t>
-  </si>
-  <si>
-    <t>2022-07-15 15:13:27.348214</t>
-  </si>
-  <si>
-    <t>157.09317634943778</t>
-  </si>
-  <si>
-    <t>(1273.5, 540.0)</t>
-  </si>
-  <si>
-    <t>180.7242374447877</t>
-  </si>
-  <si>
-    <t>(1038, 523)</t>
-  </si>
-  <si>
-    <t>(1287, 486)</t>
-  </si>
-  <si>
-    <t>251.73398658107334</t>
-  </si>
-  <si>
-    <t>0:00:00.621378</t>
-  </si>
-  <si>
-    <t>[[1067, 512, datetime.timedelta(microseconds=81938), 160.24505742125305], [1114, 510, datetime.timedelta(microseconds=164523), 121.04491592989531, -238.26541876429278], [1216, 507, datetime.timedelta(microseconds=250489), 172.4573631309366, 205.24832308421253], [1227, 499, datetime.timedelta(microseconds=346485), 16.618196599269826, -449.77175500141936], [1253, 494, datetime.timedelta(microseconds=442484), 25.330508243596956, 19.689551812782227], [1287, 489, datetime.timedelta(microseconds=538484), 27.016843771710054, 3.131635346849856]]</t>
-  </si>
-  <si>
-    <t>2022-07-15 15:13:32.185694</t>
-  </si>
-  <si>
-    <t>106.56738765265439</t>
-  </si>
-  <si>
-    <t>hit</t>
-  </si>
-  <si>
-    <t>55.66192594583842</t>
+    <t>(385.5, 360.0)</t>
+  </si>
+  <si>
+    <t>82.31190679361036</t>
+  </si>
+  <si>
+    <t>(740, 311)</t>
+  </si>
+  <si>
+    <t>(789, 294)</t>
+  </si>
+  <si>
+    <t>51.86520991955976</t>
+  </si>
+  <si>
+    <t>0:00:00.265873</t>
+  </si>
+  <si>
+    <t>[[791, 294, datetime.timedelta(microseconds=128906), 56.25456306219969]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 13:22:37.459518</t>
+  </si>
+  <si>
+    <t>15.936004015606668</t>
+  </si>
+  <si>
+    <t>123.59712779834328</t>
+  </si>
+  <si>
+    <t>(772, 308)</t>
+  </si>
+  <si>
+    <t>(809, 314)</t>
+  </si>
+  <si>
+    <t>37.48332962798263</t>
+  </si>
+  <si>
+    <t>0:00:00.407476</t>
+  </si>
+  <si>
+    <t>[[809, 308, datetime.timedelta(microseconds=145702), 78.02602838050798], [809, 314, datetime.timedelta(microseconds=280409), 6.574497919456132, -254.81183008053185]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 13:22:50.890073</t>
+  </si>
+  <si>
+    <t>11.517055313114017</t>
+  </si>
+  <si>
+    <t>96.20940702446929</t>
   </si>
   <si>
     <t>Subject Code:</t>
@@ -465,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,42 +582,42 @@
         <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>37</v>
@@ -605,6 +629,38 @@
       </c>
       <c r="B5" t="s">
         <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redid an edit on version2.py due to previous commit error
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Start</t>
   </si>
@@ -46,118 +46,94 @@
     <t>Distance From Center</t>
   </si>
   <si>
-    <t>(726, 347)</t>
-  </si>
-  <si>
-    <t>(840, 341)</t>
-  </si>
-  <si>
-    <t>114.15778554264269</t>
-  </si>
-  <si>
-    <t>0:00:00.242883</t>
-  </si>
-  <si>
-    <t>[[837, 339, datetime.timedelta(microseconds=108936), 203.11786467979857]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 13:22:23.360727</t>
-  </si>
-  <si>
-    <t>35.07590023527973</t>
+    <t>(547, 362)</t>
+  </si>
+  <si>
+    <t>(484, 381)</t>
+  </si>
+  <si>
+    <t>65.80273550544841</t>
+  </si>
+  <si>
+    <t>0:00:00.690796</t>
+  </si>
+  <si>
+    <t>[[505, 373, datetime.timedelta(microseconds=136001), 200.84810798557422], [492, 371, datetime.timedelta(microseconds=277003), 21.796434777706118, -646.3889315562218], [486, 385, datetime.timedelta(microseconds=420800), 16.61556618107878, -12.311950087042153], [484, 381, datetime.timedelta(microseconds=565304), 3.631447940954, -22.968382038911415]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 13:59:41.543855</t>
+  </si>
+  <si>
+    <t>30.205834009127525</t>
+  </si>
+  <si>
+    <t>miss</t>
+  </si>
+  <si>
+    <t>(428.0, 360.0)</t>
+  </si>
+  <si>
+    <t>59.80802621722272</t>
+  </si>
+  <si>
+    <t>(710, 375)</t>
+  </si>
+  <si>
+    <t>(844, 415)</t>
+  </si>
+  <si>
+    <t>139.84276885130672</t>
+  </si>
+  <si>
+    <t>0:00:00.590395</t>
+  </si>
+  <si>
+    <t>[[796, 406, datetime.timedelta(microseconds=208394), 537.4530806935257], [842, 415, datetime.timedelta(microseconds=420094), 51.217152911941916, -1157.4455426204227]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 13:59:48.176819</t>
+  </si>
+  <si>
+    <t>64.19288546066008</t>
   </si>
   <si>
     <t>hit</t>
   </si>
   <si>
-    <t>(893.5, 360.0)</t>
-  </si>
-  <si>
-    <t>56.77367347635698</t>
-  </si>
-  <si>
-    <t>(614, 327)</t>
-  </si>
-  <si>
-    <t>(460, 325)</t>
-  </si>
-  <si>
-    <t>154.01298646542764</t>
-  </si>
-  <si>
-    <t>0:00:00.502601</t>
-  </si>
-  <si>
-    <t>[[563, 322, datetime.timedelta(microseconds=147599), 436.052055827327], [487, 321, datetime.timedelta(microseconds=254267), 91.84689421110689, -1353.7154314803738], [462, 325, datetime.timedelta(microseconds=387026), 20.099819797663816, -185.3805026366267]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 13:22:30.539934</t>
-  </si>
-  <si>
-    <t>47.321732131716075</t>
-  </si>
-  <si>
-    <t>miss</t>
-  </si>
-  <si>
-    <t>(385.5, 360.0)</t>
-  </si>
-  <si>
-    <t>82.31190679361036</t>
-  </si>
-  <si>
-    <t>(740, 311)</t>
-  </si>
-  <si>
-    <t>(789, 294)</t>
-  </si>
-  <si>
-    <t>51.86520991955976</t>
-  </si>
-  <si>
-    <t>0:00:00.265873</t>
-  </si>
-  <si>
-    <t>[[791, 294, datetime.timedelta(microseconds=128906), 56.25456306219969]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 13:22:37.459518</t>
-  </si>
-  <si>
-    <t>15.936004015606668</t>
-  </si>
-  <si>
-    <t>123.59712779834328</t>
-  </si>
-  <si>
-    <t>(772, 308)</t>
-  </si>
-  <si>
-    <t>(809, 314)</t>
-  </si>
-  <si>
-    <t>37.48332962798263</t>
-  </si>
-  <si>
-    <t>0:00:00.407476</t>
-  </si>
-  <si>
-    <t>[[809, 308, datetime.timedelta(microseconds=145702), 78.02602838050798], [809, 314, datetime.timedelta(microseconds=280409), 6.574497919456132, -254.81183008053185]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 13:22:50.890073</t>
-  </si>
-  <si>
-    <t>11.517055313114017</t>
-  </si>
-  <si>
-    <t>96.20940702446929</t>
+    <t>(852.0, 360.0)</t>
+  </si>
+  <si>
+    <t>55.57877292636101</t>
+  </si>
+  <si>
+    <t>(559, 348)</t>
+  </si>
+  <si>
+    <t>(678, 227)</t>
+  </si>
+  <si>
+    <t>169.7115199389835</t>
+  </si>
+  <si>
+    <t>0:00:03.796694</t>
+  </si>
+  <si>
+    <t>[[477, 323, datetime.timedelta(microseconds=161609), 243.4980367780814], [381, 318, datetime.timedelta(microseconds=330717), 133.4288824928215, -332.8197651927779], [362, 321, datetime.timedelta(microseconds=488226), 18.085346825348815, -236.25029324016475], [362, 335, datetime.timedelta(microseconds=637561), 10.079829261978675, -12.55647312707355], [360, 319, datetime.timedelta(microseconds=792517), 9.339528901905195, -0.9341129087117122], [362, 327, datetime.timedelta(microseconds=934024), 4.052689245828128, -5.660282451068782], [360, 321, datetime.timedelta(seconds=1, microseconds=77222), 37.5954972730523, 434.3685481757035], [362, 335, datetime.timedelta(seconds=1, microseconds=222800), 29.137124833128706, -37.963969658543974], [509, 327, datetime.timedelta(seconds=1, microseconds=373520), 180.92248235523147, 406.36473956442165], [691, 381, datetime.timedelta(seconds=1, microseconds=662303), 131.5777792603786, -74.50472532187362], [465, 325, datetime.timedelta(seconds=1, microseconds=806844), 132.46618361503576, 1.101085655538313], [318, 275, datetime.timedelta(seconds=1, microseconds=956519), 74.51485842321786, -60.5856498321705], [459, 270, datetime.timedelta(seconds=2, microseconds=113482), 570.7052950603302, 4372.415331392753], [772, 319, datetime.timedelta(seconds=2, microseconds=271750), 535.154636715102, -130.8211898628451], [632, 291, datetime.timedelta(seconds=2, microseconds=419753), 156.1341056339755, -902.9608628910967], [296, 241, datetime.timedelta(seconds=2, microseconds=609953), 255.6500541923768, 163.1534701172079], [413, 132, datetime.timedelta(seconds=2, microseconds=775720), 94.62529763159239, -207.5810299602749], [683, 199, datetime.timedelta(seconds=2, microseconds=928935), 137.4678607749794, 46.12008713568444], [670, 212, datetime.timedelta(seconds=3, microseconds=80827), 104.4116054866245, -408.9754078260349], [658, 233, datetime.timedelta(seconds=3, microseconds=221791), 50.058853335468065, -245.06292929449992], [683, 239, datetime.timedelta(seconds=3, microseconds=363827), 32.437896790424865, -48.43223989710275], [672, 224, datetime.timedelta(seconds=3, microseconds=504925), 16.910562681868615, -30.751763348133387], [676, 224, datetime.timedelta(seconds=3, microseconds=654045), 2.8073673498203537, -21.563035161263006]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 14:00:03.569802</t>
+  </si>
+  <si>
+    <t>77.90372180331653</t>
+  </si>
+  <si>
+    <t>283.17662332897464</t>
   </si>
   <si>
     <t>Subject Code:</t>
   </si>
   <si>
-    <t>1</t>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -489,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -614,7 +590,7 @@
         <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -629,38 +605,6 @@
       </c>
       <c r="B5" t="s">
         <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
program crashed if started in center, fixed
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Start</t>
   </si>
@@ -46,88 +46,106 @@
     <t>Distance From Center</t>
   </si>
   <si>
-    <t>(547, 362)</t>
-  </si>
-  <si>
-    <t>(484, 381)</t>
-  </si>
-  <si>
-    <t>65.80273550544841</t>
-  </si>
-  <si>
-    <t>0:00:00.690796</t>
-  </si>
-  <si>
-    <t>[[505, 373, datetime.timedelta(microseconds=136001), 200.84810798557422], [492, 371, datetime.timedelta(microseconds=277003), 21.796434777706118, -646.3889315562218], [486, 385, datetime.timedelta(microseconds=420800), 16.61556618107878, -12.311950087042153], [484, 381, datetime.timedelta(microseconds=565304), 3.631447940954, -22.968382038911415]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 13:59:41.543855</t>
-  </si>
-  <si>
-    <t>30.205834009127525</t>
-  </si>
-  <si>
-    <t>miss</t>
-  </si>
-  <si>
-    <t>(428.0, 360.0)</t>
-  </si>
-  <si>
-    <t>59.80802621722272</t>
-  </si>
-  <si>
-    <t>(710, 375)</t>
-  </si>
-  <si>
-    <t>(844, 415)</t>
-  </si>
-  <si>
-    <t>139.84276885130672</t>
-  </si>
-  <si>
-    <t>0:00:00.590395</t>
-  </si>
-  <si>
-    <t>[[796, 406, datetime.timedelta(microseconds=208394), 537.4530806935257], [842, 415, datetime.timedelta(microseconds=420094), 51.217152911941916, -1157.4455426204227]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 13:59:48.176819</t>
-  </si>
-  <si>
-    <t>64.19288546066008</t>
+    <t>(564, 367)</t>
+  </si>
+  <si>
+    <t>(379, 371)</t>
+  </si>
+  <si>
+    <t>185.04323819042943</t>
+  </si>
+  <si>
+    <t>0:00:01.225507</t>
+  </si>
+  <si>
+    <t>[[479, 367, datetime.timedelta(microseconds=116545), 416.9553640327558], [427, 362, datetime.timedelta(microseconds=233742), 105.12474828050938, -1334.0803781615905], [387, 367, datetime.timedelta(microseconds=347788), 54.51952285715116, -145.50595599433626], [383, 360, datetime.timedelta(microseconds=460534), 8.234456442061992, -100.50303867920537], [379, 371, datetime.timedelta(microseconds=568476), 9.684743123859638, 2.551183659112515], [381, 367, datetime.timedelta(microseconds=684748), 3.072021014299863, -9.657161626700297], [381, 373, datetime.timedelta(microseconds=794539), 3.5520247869798998, 0.6041286490405591], [379, 369, datetime.timedelta(microseconds=910617), 2.3100384085733103, -1.3638954449637877], [381, 365, datetime.timedelta(seconds=1, microseconds=17284), 121.70563790209458, 6907.8685196436745], [381, 371, datetime.timedelta(seconds=1, microseconds=116432), 24.23923167361398, -837.1101263267882]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 14:08:43.849793</t>
+  </si>
+  <si>
+    <t>87.03885648216496</t>
   </si>
   <si>
     <t>hit</t>
   </si>
   <si>
-    <t>(852.0, 360.0)</t>
-  </si>
-  <si>
-    <t>55.57877292636101</t>
-  </si>
-  <si>
-    <t>(559, 348)</t>
-  </si>
-  <si>
-    <t>(678, 227)</t>
-  </si>
-  <si>
-    <t>169.7115199389835</t>
-  </si>
-  <si>
-    <t>0:00:03.796694</t>
-  </si>
-  <si>
-    <t>[[477, 323, datetime.timedelta(microseconds=161609), 243.4980367780814], [381, 318, datetime.timedelta(microseconds=330717), 133.4288824928215, -332.8197651927779], [362, 321, datetime.timedelta(microseconds=488226), 18.085346825348815, -236.25029324016475], [362, 335, datetime.timedelta(microseconds=637561), 10.079829261978675, -12.55647312707355], [360, 319, datetime.timedelta(microseconds=792517), 9.339528901905195, -0.9341129087117122], [362, 327, datetime.timedelta(microseconds=934024), 4.052689245828128, -5.660282451068782], [360, 321, datetime.timedelta(seconds=1, microseconds=77222), 37.5954972730523, 434.3685481757035], [362, 335, datetime.timedelta(seconds=1, microseconds=222800), 29.137124833128706, -37.963969658543974], [509, 327, datetime.timedelta(seconds=1, microseconds=373520), 180.92248235523147, 406.36473956442165], [691, 381, datetime.timedelta(seconds=1, microseconds=662303), 131.5777792603786, -74.50472532187362], [465, 325, datetime.timedelta(seconds=1, microseconds=806844), 132.46618361503576, 1.101085655538313], [318, 275, datetime.timedelta(seconds=1, microseconds=956519), 74.51485842321786, -60.5856498321705], [459, 270, datetime.timedelta(seconds=2, microseconds=113482), 570.7052950603302, 4372.415331392753], [772, 319, datetime.timedelta(seconds=2, microseconds=271750), 535.154636715102, -130.8211898628451], [632, 291, datetime.timedelta(seconds=2, microseconds=419753), 156.1341056339755, -902.9608628910967], [296, 241, datetime.timedelta(seconds=2, microseconds=609953), 255.6500541923768, 163.1534701172079], [413, 132, datetime.timedelta(seconds=2, microseconds=775720), 94.62529763159239, -207.5810299602749], [683, 199, datetime.timedelta(seconds=2, microseconds=928935), 137.4678607749794, 46.12008713568444], [670, 212, datetime.timedelta(seconds=3, microseconds=80827), 104.4116054866245, -408.9754078260349], [658, 233, datetime.timedelta(seconds=3, microseconds=221791), 50.058853335468065, -245.06292929449992], [683, 239, datetime.timedelta(seconds=3, microseconds=363827), 32.437896790424865, -48.43223989710275], [672, 224, datetime.timedelta(seconds=3, microseconds=504925), 16.910562681868615, -30.751763348133387], [676, 224, datetime.timedelta(seconds=3, microseconds=654045), 2.8073673498203537, -21.563035161263006]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 14:00:03.569802</t>
-  </si>
-  <si>
-    <t>77.90372180331653</t>
-  </si>
-  <si>
-    <t>283.17662332897464</t>
+    <t>(416.0, 360.0)</t>
+  </si>
+  <si>
+    <t>38.600518131237564</t>
+  </si>
+  <si>
+    <t>(576, 358)</t>
+  </si>
+  <si>
+    <t>(416, 369)</t>
+  </si>
+  <si>
+    <t>160.37767924496225</t>
+  </si>
+  <si>
+    <t>0:00:00.466837</t>
+  </si>
+  <si>
+    <t>[[516, 354, datetime.timedelta(microseconds=119004), 273.7557543048282], [458, 367, datetime.timedelta(microseconds=231039), 121.01145404937245, -661.1191195229193], [418, 367, datetime.timedelta(microseconds=344831), 54.5624227949773, -192.70028290494517]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 14:08:51.289994</t>
+  </si>
+  <si>
+    <t>75.43690838559337</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>(593, 377)</t>
+  </si>
+  <si>
+    <t>(454, 371)</t>
+  </si>
+  <si>
+    <t>139.12943613772032</t>
+  </si>
+  <si>
+    <t>0:00:00.562122</t>
+  </si>
+  <si>
+    <t>[[555, 375, datetime.timedelta(microseconds=122082), 104.02843990105013], [485, 371, datetime.timedelta(microseconds=232791), 141.6705917678617, 161.69934347466858], [458, 373, datetime.timedelta(microseconds=343206), 37.105396134542076, -304.671817023361], [454, 373, datetime.timedelta(microseconds=452708), 4.156059715051383, -72.78275714034365]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 14:08:57.435283</t>
+  </si>
+  <si>
+    <t>65.44236440552031</t>
+  </si>
+  <si>
+    <t>39.56008088970496</t>
+  </si>
+  <si>
+    <t>(582, 375)</t>
+  </si>
+  <si>
+    <t>(437, 369)</t>
+  </si>
+  <si>
+    <t>145.1240848377691</t>
+  </si>
+  <si>
+    <t>0:00:00.539133</t>
+  </si>
+  <si>
+    <t>[[512, 369, datetime.timedelta(microseconds=95883), 344.6560595914215], [468, 367, datetime.timedelta(microseconds=205065), 101.02975025206085, -1188.0443241867733], [441, 373, datetime.timedelta(microseconds=321080), 40.518878855951336, -188.46041919804884], [437, 367, datetime.timedelta(microseconds=424116), 7.997550145853295, -76.68026839378388]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 14:09:03.708945</t>
+  </si>
+  <si>
+    <t>68.2620695348025</t>
+  </si>
+  <si>
+    <t>22.847319317591726</t>
   </si>
   <si>
     <t>Subject Code:</t>
@@ -465,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,36 +576,36 @@
         <v>26</v>
       </c>
       <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -596,15 +614,47 @@
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big changes, fixed rectangle flashing, added timer on testing screen
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Start</t>
   </si>
@@ -46,25 +46,25 @@
     <t>Distance From Center</t>
   </si>
   <si>
-    <t>(564, 367)</t>
-  </si>
-  <si>
-    <t>(379, 371)</t>
-  </si>
-  <si>
-    <t>185.04323819042943</t>
-  </si>
-  <si>
-    <t>0:00:01.225507</t>
-  </si>
-  <si>
-    <t>[[479, 367, datetime.timedelta(microseconds=116545), 416.9553640327558], [427, 362, datetime.timedelta(microseconds=233742), 105.12474828050938, -1334.0803781615905], [387, 367, datetime.timedelta(microseconds=347788), 54.51952285715116, -145.50595599433626], [383, 360, datetime.timedelta(microseconds=460534), 8.234456442061992, -100.50303867920537], [379, 371, datetime.timedelta(microseconds=568476), 9.684743123859638, 2.551183659112515], [381, 367, datetime.timedelta(microseconds=684748), 3.072021014299863, -9.657161626700297], [381, 373, datetime.timedelta(microseconds=794539), 3.5520247869798998, 0.6041286490405591], [379, 369, datetime.timedelta(microseconds=910617), 2.3100384085733103, -1.3638954449637877], [381, 365, datetime.timedelta(seconds=1, microseconds=17284), 121.70563790209458, 6907.8685196436745], [381, 371, datetime.timedelta(seconds=1, microseconds=116432), 24.23923167361398, -837.1101263267882]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 14:08:43.849793</t>
-  </si>
-  <si>
-    <t>87.03885648216496</t>
+    <t>(585, 331)</t>
+  </si>
+  <si>
+    <t>(450, 321)</t>
+  </si>
+  <si>
+    <t>135.36986370680884</t>
+  </si>
+  <si>
+    <t>0:00:00.591743</t>
+  </si>
+  <si>
+    <t>[[553, 327, datetime.timedelta(microseconds=94817), 653.527785899376], [516, 325, datetime.timedelta(microseconds=202944), 84.83404513007834, -2802.22002507735], [481, 317, datetime.timedelta(microseconds=317487), 52.54260911975261, -101.7094747511732], [460, 319, datetime.timedelta(microseconds=413743), 23.689749565895667, -69.73618781189518], [450, 323, datetime.timedelta(microseconds=503781), 9.933409370623474, -27.306190974396007]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 16:31:25.567586</t>
+  </si>
+  <si>
+    <t>62.89746106377338</t>
   </si>
   <si>
     <t>hit</t>
@@ -73,79 +73,82 @@
     <t>(416.0, 360.0)</t>
   </si>
   <si>
-    <t>38.600518131237564</t>
-  </si>
-  <si>
-    <t>(576, 358)</t>
-  </si>
-  <si>
-    <t>(416, 369)</t>
-  </si>
-  <si>
-    <t>160.37767924496225</t>
-  </si>
-  <si>
-    <t>0:00:00.466837</t>
-  </si>
-  <si>
-    <t>[[516, 354, datetime.timedelta(microseconds=119004), 273.7557543048282], [458, 367, datetime.timedelta(microseconds=231039), 121.01145404937245, -661.1191195229193], [418, 367, datetime.timedelta(microseconds=344831), 54.5624227949773, -192.70028290494517]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 14:08:51.289994</t>
-  </si>
-  <si>
-    <t>75.43690838559337</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>(593, 377)</t>
-  </si>
-  <si>
-    <t>(454, 371)</t>
-  </si>
-  <si>
-    <t>139.12943613772032</t>
-  </si>
-  <si>
-    <t>0:00:00.562122</t>
-  </si>
-  <si>
-    <t>[[555, 375, datetime.timedelta(microseconds=122082), 104.02843990105013], [485, 371, datetime.timedelta(microseconds=232791), 141.6705917678617, 161.69934347466858], [458, 373, datetime.timedelta(microseconds=343206), 37.105396134542076, -304.671817023361], [454, 373, datetime.timedelta(microseconds=452708), 4.156059715051383, -72.78275714034365]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 14:08:57.435283</t>
-  </si>
-  <si>
-    <t>65.44236440552031</t>
-  </si>
-  <si>
-    <t>39.56008088970496</t>
-  </si>
-  <si>
-    <t>(582, 375)</t>
-  </si>
-  <si>
-    <t>(437, 369)</t>
-  </si>
-  <si>
-    <t>145.1240848377691</t>
-  </si>
-  <si>
-    <t>0:00:00.539133</t>
-  </si>
-  <si>
-    <t>[[512, 369, datetime.timedelta(microseconds=95883), 344.6560595914215], [468, 367, datetime.timedelta(microseconds=205065), 101.02975025206085, -1188.0443241867733], [441, 373, datetime.timedelta(microseconds=321080), 40.518878855951336, -188.46041919804884], [437, 367, datetime.timedelta(microseconds=424116), 7.997550145853295, -76.68026839378388]]</t>
-  </si>
-  <si>
-    <t>2022-07-18 14:09:03.708945</t>
-  </si>
-  <si>
-    <t>68.2620695348025</t>
-  </si>
-  <si>
-    <t>22.847319317591726</t>
+    <t>51.73973328110612</t>
+  </si>
+  <si>
+    <t>(672, 350)</t>
+  </si>
+  <si>
+    <t>(823, 389)</t>
+  </si>
+  <si>
+    <t>155.95512174981621</t>
+  </si>
+  <si>
+    <t>0:00:00.620233</t>
+  </si>
+  <si>
+    <t>[[700, 356, datetime.timedelta(microseconds=96082), 79.75419590077422], [739, 364, datetime.timedelta(microseconds=188565), 98.0990205156307, 97.28647742081765], [764, 364, datetime.timedelta(microseconds=305908), 37.97172240849074, -196.55353278482406], [799, 379, datetime.timedelta(microseconds=418501), 42.27646093764834, 10.286088991800728], [823, 391, datetime.timedelta(microseconds=511787), 24.36060789087095, -35.00646371786972]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 16:31:31.739858</t>
+  </si>
+  <si>
+    <t>72.46207486180485</t>
+  </si>
+  <si>
+    <t>(864.0, 360.0)</t>
+  </si>
+  <si>
+    <t>50.21951811795888</t>
+  </si>
+  <si>
+    <t>(723, 350)</t>
+  </si>
+  <si>
+    <t>(827, 385)</t>
+  </si>
+  <si>
+    <t>109.73149046650191</t>
+  </si>
+  <si>
+    <t>0:00:00.484416</t>
+  </si>
+  <si>
+    <t>[[778, 362, datetime.timedelta(microseconds=95326), 460.75635450464534], [825, 364, datetime.timedelta(microseconds=196310), 111.34209974754187, -1779.9106248133235], [823, 393, datetime.timedelta(microseconds=291252), 46.373573285444444, -223.0663702295518], [827, 385, datetime.timedelta(microseconds=386315), 10.75757903148568, -92.19417898336529]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 16:31:38.012506</t>
+  </si>
+  <si>
+    <t>50.98499739967954</t>
+  </si>
+  <si>
+    <t>44.654227123532216</t>
+  </si>
+  <si>
+    <t>(684, 352)</t>
+  </si>
+  <si>
+    <t>(844, 397)</t>
+  </si>
+  <si>
+    <t>166.20770138594662</t>
+  </si>
+  <si>
+    <t>0:00:00.606460</t>
+  </si>
+  <si>
+    <t>[[715, 366, datetime.timedelta(microseconds=113997), 138.6386690320643], [751, 352, datetime.timedelta(microseconds=207464), 86.50730606838702, -251.27907956887603], [784, 395, datetime.timedelta(microseconds=304395), 82.73694952238448, -12.386394474293422], [817, 397, datetime.timedelta(microseconds=403527), 38.06699592250878, -110.69879735402017], [842, 397, datetime.timedelta(microseconds=505468), 22.980393731228453, -29.846799780164773]]</t>
+  </si>
+  <si>
+    <t>2022-07-18 16:31:44.202323</t>
+  </si>
+  <si>
+    <t>77.22577344883618</t>
+  </si>
+  <si>
+    <t>42.05948168962618</t>
   </si>
   <si>
     <t>Subject Code:</t>
@@ -579,82 +582,82 @@
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>